<commit_message>
Adds cache dir. tslm runs
</commit_message>
<xml_diff>
--- a/reports/data_dictionary.xlsx
+++ b/reports/data_dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="shop_id_monthlvl" sheetId="1" r:id="rId1"/>
@@ -495,6 +495,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F61" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
   <autoFilter ref="A1:F61"/>
+  <sortState ref="A2:F61">
+    <sortCondition ref="E1:E61"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" name="shop_id" dataDxfId="5"/>
     <tableColumn id="2" name="loc_lvl1" dataDxfId="4"/>
@@ -772,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A16" sqref="A14:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -838,91 +841,103 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1"/>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1"/>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="F6" t="s">
-        <v>93</v>
+      <c r="E6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1"/>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D8" s="1"/>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="D9" s="1"/>
-      <c r="F9" t="s">
-        <v>93</v>
+      <c r="E9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" t="s">
@@ -931,43 +946,43 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="F12" t="s">
-        <v>94</v>
+      <c r="E12" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
@@ -976,25 +991,28 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D14" s="1"/>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" t="s">
@@ -1003,151 +1021,158 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="F16" t="s">
-        <v>95</v>
+      <c r="E16" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="1"/>
+      <c r="A17">
+        <v>36</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="2">
+        <v>42278</v>
+      </c>
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1"/>
-      <c r="F18" t="s">
-        <v>95</v>
+      <c r="E18" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="D20" s="3">
+        <v>41395</v>
+      </c>
+      <c r="E20" t="s">
+        <v>99</v>
+      </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D23" s="1"/>
+      <c r="F23" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="D26" s="1"/>
       <c r="F26" t="s">
@@ -1156,422 +1181,400 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1"/>
+      <c r="F27" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" t="s">
-        <v>91</v>
+      <c r="F29" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" t="s">
-        <v>91</v>
+      <c r="F31" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
+        <v>22</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>24</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="F36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>25</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D35" s="1"/>
-      <c r="E35" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>26</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>28</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>31</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D41" s="3">
         <v>41821</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>37</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="2">
-        <v>42278</v>
-      </c>
-      <c r="E38" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C39" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B44" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D45" s="3">
         <v>41671</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
-      <c r="B42" s="1" t="s">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>41</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>43</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D45" s="1"/>
-      <c r="E45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B48" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D52" s="3">
         <v>41699</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>49</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D51" s="3">
-        <v>41579</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>50</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="3">
+        <v>41579</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>50</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>51</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B56" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C56" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="E56" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" s="3">
-        <v>41395</v>
-      </c>
-      <c r="E57" t="s">
-        <v>99</v>
-      </c>
-      <c r="F57" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1583,7 +1586,7 @@
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1611,7 +1614,7 @@
         <v>41334</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>

</xml_diff>